<commit_message>
final project data adding aehi
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">iso_sg_avg.sim</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">ppbmi.sim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aehi.sim</t>
   </si>
   <si>
     <t xml:space="preserve">mat_educ.sim</t>
@@ -434,6 +437,9 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -470,7 +476,7 @@
         <v>22.147531322017</v>
       </c>
       <c r="L2" t="n">
-        <v>4</v>
+        <v>-0.120727216279586</v>
       </c>
       <c r="M2" t="n">
         <v>2</v>
@@ -479,6 +485,9 @@
         <v>2</v>
       </c>
       <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -517,15 +526,18 @@
         <v>36.9408784556658</v>
       </c>
       <c r="L3" t="n">
-        <v>4</v>
+        <v>2.75130514839873</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -564,15 +576,18 @@
         <v>23.5519285321819</v>
       </c>
       <c r="L4" t="n">
-        <v>3</v>
+        <v>2.83362724818019</v>
       </c>
       <c r="M4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O4" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -611,16 +626,19 @@
         <v>26.6380921983984</v>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>-0.37195726065211</v>
       </c>
       <c r="M5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O5" t="n">
         <v>2</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -658,15 +676,18 @@
         <v>28.771781133876</v>
       </c>
       <c r="L6" t="n">
+        <v>2.61762177558684</v>
+      </c>
+      <c r="M6" t="n">
         <v>3</v>
       </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
       <c r="N6" t="n">
         <v>2</v>
       </c>
       <c r="O6" t="n">
+        <v>2</v>
+      </c>
+      <c r="P6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -705,15 +726,18 @@
         <v>21.1422876883203</v>
       </c>
       <c r="L7" t="n">
-        <v>2</v>
+        <v>1.04746382505513</v>
       </c>
       <c r="M7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" t="n">
+        <v>2</v>
+      </c>
+      <c r="P7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -752,15 +776,18 @@
         <v>26.2045341543511</v>
       </c>
       <c r="L8" t="n">
+        <v>4.15413698889687</v>
+      </c>
+      <c r="M8" t="n">
         <v>4</v>
       </c>
-      <c r="M8" t="n">
-        <v>1</v>
-      </c>
       <c r="N8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O8" t="n">
+        <v>1</v>
+      </c>
+      <c r="P8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -799,15 +826,18 @@
         <v>23.436702460793</v>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>0.704233888771307</v>
       </c>
       <c r="M9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N9" t="n">
         <v>2</v>
       </c>
       <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -846,15 +876,18 @@
         <v>29.5843763893029</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>-0.026595776224698</v>
       </c>
       <c r="M10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O10" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -893,16 +926,19 @@
         <v>25.8746118968263</v>
       </c>
       <c r="L11" t="n">
+        <v>4.47734646679171</v>
+      </c>
+      <c r="M11" t="n">
         <v>3</v>
       </c>
-      <c r="M11" t="n">
-        <v>1</v>
-      </c>
       <c r="N11" t="n">
         <v>1</v>
       </c>
       <c r="O11" t="n">
         <v>2</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -940,15 +976,18 @@
         <v>27.1731775971305</v>
       </c>
       <c r="L12" t="n">
-        <v>4</v>
+        <v>1.64937131515771</v>
       </c>
       <c r="M12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N12" t="n">
         <v>2</v>
       </c>
       <c r="O12" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -987,15 +1026,18 @@
         <v>25.5479833123737</v>
       </c>
       <c r="L13" t="n">
-        <v>4</v>
+        <v>2.48157371941218</v>
       </c>
       <c r="M13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O13" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1034,15 +1076,18 @@
         <v>18.5794857613929</v>
       </c>
       <c r="L14" t="n">
+        <v>2.28624762537304</v>
+      </c>
+      <c r="M14" t="n">
         <v>3</v>
       </c>
-      <c r="M14" t="n">
-        <v>2</v>
-      </c>
       <c r="N14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1081,15 +1126,18 @@
         <v>14.9560307942167</v>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>5.13027438047957</v>
       </c>
       <c r="M15" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" t="n">
+        <v>1</v>
+      </c>
+      <c r="P15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1128,16 +1176,19 @@
         <v>27.9400891223001</v>
       </c>
       <c r="L16" t="n">
+        <v>2.018583558953</v>
+      </c>
+      <c r="M16" t="n">
         <v>4</v>
       </c>
-      <c r="M16" t="n">
-        <v>2</v>
-      </c>
       <c r="N16" t="n">
         <v>1</v>
       </c>
       <c r="O16" t="n">
         <v>1</v>
+      </c>
+      <c r="P16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1175,15 +1226,18 @@
         <v>37.8655007394397</v>
       </c>
       <c r="L17" t="n">
-        <v>3</v>
+        <v>1.63139151207153</v>
       </c>
       <c r="M17" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" t="n">
+        <v>1</v>
+      </c>
+      <c r="P17" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1222,15 +1276,18 @@
         <v>22.1101190350155</v>
       </c>
       <c r="L18" t="n">
+        <v>6.08040191880039</v>
+      </c>
+      <c r="M18" t="n">
         <v>4</v>
       </c>
-      <c r="M18" t="n">
-        <v>2</v>
-      </c>
       <c r="N18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" t="n">
+        <v>1</v>
+      </c>
+      <c r="P18" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1269,15 +1326,18 @@
         <v>26.3037444172265</v>
       </c>
       <c r="L19" t="n">
-        <v>4</v>
+        <v>3.14268306341866</v>
       </c>
       <c r="M19" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N19" t="n">
         <v>2</v>
       </c>
       <c r="O19" t="n">
+        <v>1</v>
+      </c>
+      <c r="P19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1316,16 +1376,19 @@
         <v>22.9681335979242</v>
       </c>
       <c r="L20" t="n">
-        <v>2</v>
+        <v>3.73253142396558</v>
       </c>
       <c r="M20" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O20" t="n">
         <v>1</v>
+      </c>
+      <c r="P20" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1363,15 +1426,18 @@
         <v>23.3485738635826</v>
       </c>
       <c r="L21" t="n">
-        <v>3</v>
+        <v>2.10155606274561</v>
       </c>
       <c r="M21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O21" t="n">
+        <v>1</v>
+      </c>
+      <c r="P21" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1410,15 +1476,18 @@
         <v>24.1948117293095</v>
       </c>
       <c r="L22" t="n">
-        <v>4</v>
+        <v>-2.07203533900609</v>
       </c>
       <c r="M22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O22" t="n">
+        <v>1</v>
+      </c>
+      <c r="P22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1457,15 +1526,18 @@
         <v>21.9430569426347</v>
       </c>
       <c r="L23" t="n">
+        <v>3.28854917757114</v>
+      </c>
+      <c r="M23" t="n">
         <v>4</v>
       </c>
-      <c r="M23" t="n">
-        <v>2</v>
-      </c>
       <c r="N23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" t="n">
+        <v>1</v>
+      </c>
+      <c r="P23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1504,16 +1576,19 @@
         <v>14.0318289861559</v>
       </c>
       <c r="L24" t="n">
+        <v>1.03585347757644</v>
+      </c>
+      <c r="M24" t="n">
         <v>3</v>
       </c>
-      <c r="M24" t="n">
-        <v>2</v>
-      </c>
       <c r="N24" t="n">
         <v>1</v>
       </c>
       <c r="O24" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -1551,15 +1626,18 @@
         <v>27.2236231927017</v>
       </c>
       <c r="L25" t="n">
-        <v>3</v>
+        <v>-0.416506632590279</v>
       </c>
       <c r="M25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N25" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O25" t="n">
+        <v>1</v>
+      </c>
+      <c r="P25" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1598,16 +1676,19 @@
         <v>18.713754608633</v>
       </c>
       <c r="L26" t="n">
+        <v>1.2448262114158</v>
+      </c>
+      <c r="M26" t="n">
         <v>4</v>
       </c>
-      <c r="M26" t="n">
-        <v>2</v>
-      </c>
       <c r="N26" t="n">
         <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1645,16 +1726,19 @@
         <v>22.2970711871228</v>
       </c>
       <c r="L27" t="n">
-        <v>3</v>
+        <v>3.32916332367936</v>
       </c>
       <c r="M27" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N27" t="n">
         <v>1</v>
       </c>
       <c r="O27" t="n">
         <v>2</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1692,15 +1776,18 @@
         <v>23.9056608880301</v>
       </c>
       <c r="L28" t="n">
-        <v>2</v>
+        <v>3.14775148667151</v>
       </c>
       <c r="M28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O28" t="n">
+        <v>1</v>
+      </c>
+      <c r="P28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1739,16 +1826,19 @@
         <v>25.1814708296314</v>
       </c>
       <c r="L29" t="n">
+        <v>2.81168014182954</v>
+      </c>
+      <c r="M29" t="n">
         <v>4</v>
       </c>
-      <c r="M29" t="n">
-        <v>2</v>
-      </c>
       <c r="N29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O29" t="n">
         <v>1</v>
+      </c>
+      <c r="P29" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1786,16 +1876,19 @@
         <v>26.2868516468492</v>
       </c>
       <c r="L30" t="n">
+        <v>1.73205010023004</v>
+      </c>
+      <c r="M30" t="n">
         <v>4</v>
       </c>
-      <c r="M30" t="n">
-        <v>2</v>
-      </c>
       <c r="N30" t="n">
         <v>1</v>
       </c>
       <c r="O30" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P30" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1833,15 +1926,18 @@
         <v>21.5007689586757</v>
       </c>
       <c r="L31" t="n">
-        <v>3</v>
+        <v>3.15575183167477</v>
       </c>
       <c r="M31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N31" t="n">
         <v>1</v>
       </c>
       <c r="O31" t="n">
+        <v>2</v>
+      </c>
+      <c r="P31" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1880,15 +1976,18 @@
         <v>22.5214023270139</v>
       </c>
       <c r="L32" t="n">
-        <v>4</v>
+        <v>3.32061257748806</v>
       </c>
       <c r="M32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O32" t="n">
+        <v>1</v>
+      </c>
+      <c r="P32" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1927,16 +2026,19 @@
         <v>22.8132415268304</v>
       </c>
       <c r="L33" t="n">
-        <v>4</v>
+        <v>2.07511134144691</v>
       </c>
       <c r="M33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N33" t="n">
         <v>1</v>
       </c>
       <c r="O33" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P33" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1974,15 +2076,18 @@
         <v>25.5919602166096</v>
       </c>
       <c r="L34" t="n">
-        <v>2</v>
+        <v>1.00616044328192</v>
       </c>
       <c r="M34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O34" t="n">
+        <v>1</v>
+      </c>
+      <c r="P34" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2021,15 +2126,18 @@
         <v>25.3563261591335</v>
       </c>
       <c r="L35" t="n">
+        <v>3.75786967476753</v>
+      </c>
+      <c r="M35" t="n">
         <v>3</v>
       </c>
-      <c r="M35" t="n">
-        <v>2</v>
-      </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P35" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2068,15 +2176,18 @@
         <v>22.7964155770804</v>
       </c>
       <c r="L36" t="n">
-        <v>3</v>
+        <v>1.13384214295713</v>
       </c>
       <c r="M36" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N36" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O36" t="n">
+        <v>1</v>
+      </c>
+      <c r="P36" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2115,15 +2226,18 @@
         <v>27.313679568659</v>
       </c>
       <c r="L37" t="n">
+        <v>1.53022204406208</v>
+      </c>
+      <c r="M37" t="n">
         <v>3</v>
       </c>
-      <c r="M37" t="n">
-        <v>2</v>
-      </c>
       <c r="N37" t="n">
         <v>2</v>
       </c>
       <c r="O37" t="n">
+        <v>1</v>
+      </c>
+      <c r="P37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2162,16 +2276,19 @@
         <v>27.8062575171263</v>
       </c>
       <c r="L38" t="n">
-        <v>3</v>
+        <v>0.465073745006576</v>
       </c>
       <c r="M38" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N38" t="n">
         <v>1</v>
       </c>
       <c r="O38" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P38" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -2209,7 +2326,7 @@
         <v>20.6106127146561</v>
       </c>
       <c r="L39" t="n">
-        <v>4</v>
+        <v>1.00187016361946</v>
       </c>
       <c r="M39" t="n">
         <v>2</v>
@@ -2219,6 +2336,9 @@
       </c>
       <c r="O39" t="n">
         <v>1</v>
+      </c>
+      <c r="P39" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -2256,16 +2376,19 @@
         <v>29.7795668324478</v>
       </c>
       <c r="L40" t="n">
-        <v>4</v>
+        <v>2.01704286140995</v>
       </c>
       <c r="M40" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N40" t="n">
         <v>2</v>
       </c>
       <c r="O40" t="n">
         <v>1</v>
+      </c>
+      <c r="P40" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -2303,15 +2426,18 @@
         <v>30.0632384684085</v>
       </c>
       <c r="L41" t="n">
+        <v>1.04431625373036</v>
+      </c>
+      <c r="M41" t="n">
         <v>4</v>
       </c>
-      <c r="M41" t="n">
-        <v>2</v>
-      </c>
       <c r="N41" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O41" t="n">
+        <v>2</v>
+      </c>
+      <c r="P41" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2350,16 +2476,19 @@
         <v>32.5945864679651</v>
       </c>
       <c r="L42" t="n">
+        <v>3.81897590412</v>
+      </c>
+      <c r="M42" t="n">
         <v>4</v>
       </c>
-      <c r="M42" t="n">
-        <v>2</v>
-      </c>
       <c r="N42" t="n">
         <v>1</v>
       </c>
       <c r="O42" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P42" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -2397,16 +2526,19 @@
         <v>19.8609786567614</v>
       </c>
       <c r="L43" t="n">
-        <v>2</v>
+        <v>4.66190394772325</v>
       </c>
       <c r="M43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N43" t="n">
         <v>1</v>
       </c>
       <c r="O43" t="n">
         <v>2</v>
+      </c>
+      <c r="P43" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -2444,15 +2576,18 @@
         <v>29.614472746651</v>
       </c>
       <c r="L44" t="n">
+        <v>4.61015592087476</v>
+      </c>
+      <c r="M44" t="n">
         <v>3</v>
       </c>
-      <c r="M44" t="n">
-        <v>2</v>
-      </c>
       <c r="N44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O44" t="n">
+        <v>1</v>
+      </c>
+      <c r="P44" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2491,16 +2626,19 @@
         <v>27.4843968271632</v>
       </c>
       <c r="L45" t="n">
-        <v>4</v>
+        <v>3.66473474892553</v>
       </c>
       <c r="M45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N45" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O45" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P45" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
@@ -2538,16 +2676,19 @@
         <v>28.2433769637402</v>
       </c>
       <c r="L46" t="n">
+        <v>1.44257328476254</v>
+      </c>
+      <c r="M46" t="n">
         <v>4</v>
       </c>
-      <c r="M46" t="n">
-        <v>2</v>
-      </c>
       <c r="N46" t="n">
         <v>1</v>
       </c>
       <c r="O46" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P46" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2585,16 +2726,19 @@
         <v>25.2127085968425</v>
       </c>
       <c r="L47" t="n">
-        <v>3</v>
+        <v>1.90362769519121</v>
       </c>
       <c r="M47" t="n">
         <v>2</v>
       </c>
       <c r="N47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O47" t="n">
         <v>2</v>
+      </c>
+      <c r="P47" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -2632,15 +2776,18 @@
         <v>26.1220340896314</v>
       </c>
       <c r="L48" t="n">
+        <v>2.97105155648313</v>
+      </c>
+      <c r="M48" t="n">
         <v>4</v>
       </c>
-      <c r="M48" t="n">
-        <v>2</v>
-      </c>
       <c r="N48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O48" t="n">
+        <v>1</v>
+      </c>
+      <c r="P48" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2679,15 +2826,18 @@
         <v>24.2175297856688</v>
       </c>
       <c r="L49" t="n">
-        <v>2</v>
+        <v>2.37300134665967</v>
       </c>
       <c r="M49" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O49" t="n">
+        <v>1</v>
+      </c>
+      <c r="P49" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2726,15 +2876,18 @@
         <v>13.5787730011139</v>
       </c>
       <c r="L50" t="n">
-        <v>4</v>
+        <v>2.15261705718519</v>
       </c>
       <c r="M50" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N50" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O50" t="n">
+        <v>1</v>
+      </c>
+      <c r="P50" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2773,15 +2926,18 @@
         <v>24.846028469214</v>
       </c>
       <c r="L51" t="n">
-        <v>4</v>
+        <v>1.97662954744256</v>
       </c>
       <c r="M51" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N51" t="n">
         <v>2</v>
       </c>
       <c r="O51" t="n">
+        <v>1</v>
+      </c>
+      <c r="P51" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2820,15 +2976,18 @@
         <v>26.3825987229477</v>
       </c>
       <c r="L52" t="n">
+        <v>0.608211130378292</v>
+      </c>
+      <c r="M52" t="n">
         <v>3</v>
       </c>
-      <c r="M52" t="n">
-        <v>2</v>
-      </c>
       <c r="N52" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O52" t="n">
+        <v>1</v>
+      </c>
+      <c r="P52" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2867,15 +3026,18 @@
         <v>28.2236034924595</v>
       </c>
       <c r="L53" t="n">
-        <v>4</v>
+        <v>0.721055564894838</v>
       </c>
       <c r="M53" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O53" t="n">
+        <v>1</v>
+      </c>
+      <c r="P53" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2914,15 +3076,18 @@
         <v>30.0741181964501</v>
       </c>
       <c r="L54" t="n">
-        <v>3</v>
+        <v>1.92350680831478</v>
       </c>
       <c r="M54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N54" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O54" t="n">
+        <v>1</v>
+      </c>
+      <c r="P54" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2961,15 +3126,18 @@
         <v>28.1662761069509</v>
       </c>
       <c r="L55" t="n">
+        <v>2.95712937951758</v>
+      </c>
+      <c r="M55" t="n">
         <v>4</v>
       </c>
-      <c r="M55" t="n">
-        <v>2</v>
-      </c>
       <c r="N55" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O55" t="n">
+        <v>2</v>
+      </c>
+      <c r="P55" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3008,16 +3176,19 @@
         <v>23.6553761082958</v>
       </c>
       <c r="L56" t="n">
-        <v>3</v>
+        <v>4.63913186398905</v>
       </c>
       <c r="M56" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N56" t="n">
         <v>1</v>
       </c>
       <c r="O56" t="n">
         <v>2</v>
+      </c>
+      <c r="P56" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -3055,15 +3226,18 @@
         <v>32.552556277115</v>
       </c>
       <c r="L57" t="n">
-        <v>3</v>
+        <v>3.96256014133361</v>
       </c>
       <c r="M57" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O57" t="n">
+        <v>1</v>
+      </c>
+      <c r="P57" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3102,15 +3276,18 @@
         <v>25.538366382299</v>
       </c>
       <c r="L58" t="n">
+        <v>2.17256015722545</v>
+      </c>
+      <c r="M58" t="n">
         <v>4</v>
       </c>
-      <c r="M58" t="n">
-        <v>2</v>
-      </c>
       <c r="N58" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O58" t="n">
+        <v>2</v>
+      </c>
+      <c r="P58" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3149,15 +3326,18 @@
         <v>25.1960740480841</v>
       </c>
       <c r="L59" t="n">
-        <v>3</v>
+        <v>4.16505441983241</v>
       </c>
       <c r="M59" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N59" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O59" t="n">
+        <v>1</v>
+      </c>
+      <c r="P59" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3196,7 +3376,7 @@
         <v>28.0556282857852</v>
       </c>
       <c r="L60" t="n">
-        <v>3</v>
+        <v>0.167590188846662</v>
       </c>
       <c r="M60" t="n">
         <v>2</v>
@@ -3205,6 +3385,9 @@
         <v>2</v>
       </c>
       <c r="O60" t="n">
+        <v>2</v>
+      </c>
+      <c r="P60" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3243,15 +3426,18 @@
         <v>29.2973274652801</v>
       </c>
       <c r="L61" t="n">
+        <v>2.78289924241991</v>
+      </c>
+      <c r="M61" t="n">
         <v>4</v>
       </c>
-      <c r="M61" t="n">
-        <v>2</v>
-      </c>
       <c r="N61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O61" t="n">
+        <v>2</v>
+      </c>
+      <c r="P61" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3290,15 +3476,18 @@
         <v>16.95410435377</v>
       </c>
       <c r="L62" t="n">
+        <v>4.4594883731993</v>
+      </c>
+      <c r="M62" t="n">
         <v>3</v>
       </c>
-      <c r="M62" t="n">
-        <v>2</v>
-      </c>
       <c r="N62" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O62" t="n">
+        <v>1</v>
+      </c>
+      <c r="P62" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3337,15 +3526,18 @@
         <v>26.7789881858044</v>
       </c>
       <c r="L63" t="n">
-        <v>3</v>
+        <v>0.986816435640711</v>
       </c>
       <c r="M63" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O63" t="n">
+        <v>1</v>
+      </c>
+      <c r="P63" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3384,15 +3576,18 @@
         <v>24.4236330680113</v>
       </c>
       <c r="L64" t="n">
+        <v>1.2511045056782</v>
+      </c>
+      <c r="M64" t="n">
         <v>4</v>
       </c>
-      <c r="M64" t="n">
-        <v>2</v>
-      </c>
       <c r="N64" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O64" t="n">
+        <v>1</v>
+      </c>
+      <c r="P64" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3431,7 +3626,7 @@
         <v>33.5458517025218</v>
       </c>
       <c r="L65" t="n">
-        <v>4</v>
+        <v>0.0311085379169879</v>
       </c>
       <c r="M65" t="n">
         <v>2</v>
@@ -3440,7 +3635,10 @@
         <v>2</v>
       </c>
       <c r="O65" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="P65" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="66">
@@ -3478,15 +3676,18 @@
         <v>20.3518581810169</v>
       </c>
       <c r="L66" t="n">
+        <v>1.45209742760402</v>
+      </c>
+      <c r="M66" t="n">
         <v>4</v>
       </c>
-      <c r="M66" t="n">
-        <v>2</v>
-      </c>
       <c r="N66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O66" t="n">
+        <v>1</v>
+      </c>
+      <c r="P66" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3525,15 +3726,18 @@
         <v>33.3135933067604</v>
       </c>
       <c r="L67" t="n">
-        <v>4</v>
+        <v>3.0248385940428</v>
       </c>
       <c r="M67" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O67" t="n">
+        <v>1</v>
+      </c>
+      <c r="P67" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3572,7 +3776,7 @@
         <v>31.5585504136809</v>
       </c>
       <c r="L68" t="n">
-        <v>3</v>
+        <v>0.912827464998632</v>
       </c>
       <c r="M68" t="n">
         <v>2</v>
@@ -3581,6 +3785,9 @@
         <v>2</v>
       </c>
       <c r="O68" t="n">
+        <v>1</v>
+      </c>
+      <c r="P68" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3619,15 +3826,18 @@
         <v>27.8372471247481</v>
       </c>
       <c r="L69" t="n">
+        <v>2.04696957809666</v>
+      </c>
+      <c r="M69" t="n">
         <v>4</v>
       </c>
-      <c r="M69" t="n">
-        <v>2</v>
-      </c>
       <c r="N69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O69" t="n">
+        <v>1</v>
+      </c>
+      <c r="P69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3666,15 +3876,18 @@
         <v>28.4003423733509</v>
       </c>
       <c r="L70" t="n">
-        <v>4</v>
+        <v>1.26135381230092</v>
       </c>
       <c r="M70" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N70" t="n">
         <v>2</v>
       </c>
       <c r="O70" t="n">
+        <v>1</v>
+      </c>
+      <c r="P70" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3713,15 +3926,18 @@
         <v>23.3984012005794</v>
       </c>
       <c r="L71" t="n">
+        <v>1.94642800595254</v>
+      </c>
+      <c r="M71" t="n">
         <v>4</v>
       </c>
-      <c r="M71" t="n">
-        <v>2</v>
-      </c>
       <c r="N71" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O71" t="n">
+        <v>1</v>
+      </c>
+      <c r="P71" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3760,16 +3976,19 @@
         <v>27.618698836763</v>
       </c>
       <c r="L72" t="n">
-        <v>4</v>
+        <v>3.67200180899057</v>
       </c>
       <c r="M72" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N72" t="n">
         <v>1</v>
       </c>
       <c r="O72" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P72" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -3807,15 +4026,18 @@
         <v>32.743926263528</v>
       </c>
       <c r="L73" t="n">
+        <v>2.32436772625763</v>
+      </c>
+      <c r="M73" t="n">
         <v>4</v>
       </c>
-      <c r="M73" t="n">
-        <v>2</v>
-      </c>
       <c r="N73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O73" t="n">
+        <v>1</v>
+      </c>
+      <c r="P73" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3854,15 +4076,18 @@
         <v>31.9745166101443</v>
       </c>
       <c r="L74" t="n">
-        <v>4</v>
+        <v>2.02151966150289</v>
       </c>
       <c r="M74" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N74" t="n">
         <v>2</v>
       </c>
       <c r="O74" t="n">
+        <v>2</v>
+      </c>
+      <c r="P74" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3901,15 +4126,18 @@
         <v>23.2848471918507</v>
       </c>
       <c r="L75" t="n">
-        <v>3</v>
+        <v>1.95268149476373</v>
       </c>
       <c r="M75" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N75" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O75" t="n">
+        <v>1</v>
+      </c>
+      <c r="P75" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3948,16 +4176,19 @@
         <v>20.6783018993451</v>
       </c>
       <c r="L76" t="n">
+        <v>5.24519377663619</v>
+      </c>
+      <c r="M76" t="n">
         <v>4</v>
       </c>
-      <c r="M76" t="n">
-        <v>2</v>
-      </c>
       <c r="N76" t="n">
         <v>1</v>
       </c>
       <c r="O76" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P76" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3995,15 +4226,18 @@
         <v>27.3367452239203</v>
       </c>
       <c r="L77" t="n">
+        <v>-0.239761741463687</v>
+      </c>
+      <c r="M77" t="n">
         <v>3</v>
       </c>
-      <c r="M77" t="n">
-        <v>2</v>
-      </c>
       <c r="N77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O77" t="n">
+        <v>1</v>
+      </c>
+      <c r="P77" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4042,15 +4276,18 @@
         <v>26.815034048423</v>
       </c>
       <c r="L78" t="n">
+        <v>2.00809996190616</v>
+      </c>
+      <c r="M78" t="n">
         <v>4</v>
       </c>
-      <c r="M78" t="n">
-        <v>2</v>
-      </c>
       <c r="N78" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O78" t="n">
+        <v>1</v>
+      </c>
+      <c r="P78" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4089,16 +4326,19 @@
         <v>29.3103056433686</v>
       </c>
       <c r="L79" t="n">
-        <v>2</v>
+        <v>0.108927019289596</v>
       </c>
       <c r="M79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N79" t="n">
         <v>2</v>
       </c>
       <c r="O79" t="n">
         <v>1</v>
+      </c>
+      <c r="P79" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -4136,16 +4376,19 @@
         <v>18.1649519487032</v>
       </c>
       <c r="L80" t="n">
+        <v>0.254364380422306</v>
+      </c>
+      <c r="M80" t="n">
         <v>4</v>
       </c>
-      <c r="M80" t="n">
-        <v>2</v>
-      </c>
       <c r="N80" t="n">
         <v>1</v>
       </c>
       <c r="O80" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P80" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -4183,16 +4426,19 @@
         <v>33.2322338716174</v>
       </c>
       <c r="L81" t="n">
+        <v>4.02969248613252</v>
+      </c>
+      <c r="M81" t="n">
         <v>3</v>
       </c>
-      <c r="M81" t="n">
-        <v>2</v>
-      </c>
       <c r="N81" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O81" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P81" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -4230,16 +4476,19 @@
         <v>17.2646069999246</v>
       </c>
       <c r="L82" t="n">
+        <v>2.98499219198699</v>
+      </c>
+      <c r="M82" t="n">
         <v>3</v>
       </c>
-      <c r="M82" t="n">
-        <v>2</v>
-      </c>
       <c r="N82" t="n">
         <v>2</v>
       </c>
       <c r="O82" t="n">
         <v>1</v>
+      </c>
+      <c r="P82" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="83">
@@ -4277,15 +4526,18 @@
         <v>25.760585742984</v>
       </c>
       <c r="L83" t="n">
-        <v>4</v>
+        <v>2.62868871458903</v>
       </c>
       <c r="M83" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O83" t="n">
+        <v>1</v>
+      </c>
+      <c r="P83" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4324,15 +4576,18 @@
         <v>31.0011286245914</v>
       </c>
       <c r="L84" t="n">
-        <v>2</v>
+        <v>4.28937488784411</v>
       </c>
       <c r="M84" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O84" t="n">
+        <v>1</v>
+      </c>
+      <c r="P84" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4371,16 +4626,19 @@
         <v>19.8342341715336</v>
       </c>
       <c r="L85" t="n">
-        <v>4</v>
+        <v>0.385535035258108</v>
       </c>
       <c r="M85" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N85" t="n">
         <v>1</v>
       </c>
       <c r="O85" t="n">
         <v>2</v>
+      </c>
+      <c r="P85" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -4418,15 +4676,18 @@
         <v>21.7370984523445</v>
       </c>
       <c r="L86" t="n">
-        <v>2</v>
+        <v>0.698700525426428</v>
       </c>
       <c r="M86" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O86" t="n">
+        <v>2</v>
+      </c>
+      <c r="P86" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4465,15 +4726,18 @@
         <v>27.5232034488987</v>
       </c>
       <c r="L87" t="n">
-        <v>4</v>
+        <v>4.35851563319614</v>
       </c>
       <c r="M87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N87" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O87" t="n">
+        <v>1</v>
+      </c>
+      <c r="P87" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4512,15 +4776,18 @@
         <v>27.3585129868351</v>
       </c>
       <c r="L88" t="n">
+        <v>1.52598030968128</v>
+      </c>
+      <c r="M88" t="n">
         <v>3</v>
       </c>
-      <c r="M88" t="n">
-        <v>2</v>
-      </c>
       <c r="N88" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O88" t="n">
+        <v>1</v>
+      </c>
+      <c r="P88" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4559,15 +4826,18 @@
         <v>25.5797769334851</v>
       </c>
       <c r="L89" t="n">
-        <v>3</v>
+        <v>-0.223982611960056</v>
       </c>
       <c r="M89" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O89" t="n">
+        <v>1</v>
+      </c>
+      <c r="P89" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4606,15 +4876,18 @@
         <v>33.2526447158025</v>
       </c>
       <c r="L90" t="n">
+        <v>2.70526085427941</v>
+      </c>
+      <c r="M90" t="n">
         <v>4</v>
       </c>
-      <c r="M90" t="n">
-        <v>2</v>
-      </c>
       <c r="N90" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O90" t="n">
+        <v>1</v>
+      </c>
+      <c r="P90" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4653,15 +4926,18 @@
         <v>21.3320746952569</v>
       </c>
       <c r="L91" t="n">
-        <v>4</v>
+        <v>3.45177221183473</v>
       </c>
       <c r="M91" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N91" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O91" t="n">
+        <v>1</v>
+      </c>
+      <c r="P91" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4700,15 +4976,18 @@
         <v>23.571610983886</v>
       </c>
       <c r="L92" t="n">
-        <v>4</v>
+        <v>0.725279322864361</v>
       </c>
       <c r="M92" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O92" t="n">
+        <v>1</v>
+      </c>
+      <c r="P92" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4747,15 +5026,18 @@
         <v>29.7283262903337</v>
       </c>
       <c r="L93" t="n">
+        <v>1.43379413634421</v>
+      </c>
+      <c r="M93" t="n">
         <v>3</v>
       </c>
-      <c r="M93" t="n">
-        <v>1</v>
-      </c>
       <c r="N93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O93" t="n">
+        <v>1</v>
+      </c>
+      <c r="P93" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4794,15 +5076,18 @@
         <v>19.2749839532522</v>
       </c>
       <c r="L94" t="n">
+        <v>3.41344657495503</v>
+      </c>
+      <c r="M94" t="n">
         <v>3</v>
       </c>
-      <c r="M94" t="n">
-        <v>2</v>
-      </c>
       <c r="N94" t="n">
         <v>2</v>
       </c>
       <c r="O94" t="n">
+        <v>1</v>
+      </c>
+      <c r="P94" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4841,15 +5126,18 @@
         <v>33.545506023313</v>
       </c>
       <c r="L95" t="n">
+        <v>1.00475795740121</v>
+      </c>
+      <c r="M95" t="n">
         <v>4</v>
       </c>
-      <c r="M95" t="n">
-        <v>2</v>
-      </c>
       <c r="N95" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O95" t="n">
+        <v>1</v>
+      </c>
+      <c r="P95" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4888,16 +5176,19 @@
         <v>24.23580967074</v>
       </c>
       <c r="L96" t="n">
+        <v>2.61399454220801</v>
+      </c>
+      <c r="M96" t="n">
         <v>3</v>
       </c>
-      <c r="M96" t="n">
-        <v>2</v>
-      </c>
       <c r="N96" t="n">
         <v>2</v>
       </c>
       <c r="O96" t="n">
         <v>1</v>
+      </c>
+      <c r="P96" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="97">
@@ -4935,7 +5226,7 @@
         <v>33.1145414154597</v>
       </c>
       <c r="L97" t="n">
-        <v>4</v>
+        <v>0.0032303541847679</v>
       </c>
       <c r="M97" t="n">
         <v>2</v>
@@ -4944,6 +5235,9 @@
         <v>2</v>
       </c>
       <c r="O97" t="n">
+        <v>1</v>
+      </c>
+      <c r="P97" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4982,15 +5276,18 @@
         <v>27.4307605015339</v>
       </c>
       <c r="L98" t="n">
-        <v>4</v>
+        <v>0.867547693393099</v>
       </c>
       <c r="M98" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O98" t="n">
+        <v>1</v>
+      </c>
+      <c r="P98" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5029,15 +5326,18 @@
         <v>22.5692744908662</v>
       </c>
       <c r="L99" t="n">
+        <v>1.76385995430911</v>
+      </c>
+      <c r="M99" t="n">
         <v>4</v>
       </c>
-      <c r="M99" t="n">
-        <v>2</v>
-      </c>
       <c r="N99" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O99" t="n">
+        <v>2</v>
+      </c>
+      <c r="P99" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5076,15 +5376,18 @@
         <v>26.1350702240324</v>
       </c>
       <c r="L100" t="n">
-        <v>4</v>
+        <v>3.22973966298217</v>
       </c>
       <c r="M100" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N100" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O100" t="n">
+        <v>1</v>
+      </c>
+      <c r="P100" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5123,15 +5426,18 @@
         <v>37.1859172220774</v>
       </c>
       <c r="L101" t="n">
+        <v>3.69628448028871</v>
+      </c>
+      <c r="M101" t="n">
         <v>4</v>
       </c>
-      <c r="M101" t="n">
-        <v>2</v>
-      </c>
       <c r="N101" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O101" t="n">
+        <v>1</v>
+      </c>
+      <c r="P101" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5170,16 +5476,19 @@
         <v>32.0496045147998</v>
       </c>
       <c r="L102" t="n">
+        <v>0.977059441492458</v>
+      </c>
+      <c r="M102" t="n">
         <v>4</v>
       </c>
-      <c r="M102" t="n">
-        <v>2</v>
-      </c>
       <c r="N102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O102" t="n">
         <v>1</v>
+      </c>
+      <c r="P102" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="103">
@@ -5217,7 +5526,7 @@
         <v>26.5628798762492</v>
       </c>
       <c r="L103" t="n">
-        <v>3</v>
+        <v>-0.963004101918115</v>
       </c>
       <c r="M103" t="n">
         <v>2</v>
@@ -5226,6 +5535,9 @@
         <v>2</v>
       </c>
       <c r="O103" t="n">
+        <v>1</v>
+      </c>
+      <c r="P103" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5264,15 +5576,18 @@
         <v>16.2407330289718</v>
       </c>
       <c r="L104" t="n">
+        <v>4.28344641039364</v>
+      </c>
+      <c r="M104" t="n">
         <v>4</v>
       </c>
-      <c r="M104" t="n">
-        <v>1</v>
-      </c>
       <c r="N104" t="n">
         <v>1</v>
       </c>
       <c r="O104" t="n">
+        <v>1</v>
+      </c>
+      <c r="P104" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5311,15 +5626,18 @@
         <v>21.1791171922604</v>
       </c>
       <c r="L105" t="n">
+        <v>3.1377544762223</v>
+      </c>
+      <c r="M105" t="n">
         <v>4</v>
       </c>
-      <c r="M105" t="n">
-        <v>2</v>
-      </c>
       <c r="N105" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O105" t="n">
+        <v>1</v>
+      </c>
+      <c r="P105" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5358,15 +5676,18 @@
         <v>29.7741945042642</v>
       </c>
       <c r="L106" t="n">
-        <v>4</v>
+        <v>-0.604612953579649</v>
       </c>
       <c r="M106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O106" t="n">
+        <v>1</v>
+      </c>
+      <c r="P106" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5405,15 +5726,18 @@
         <v>20.097549302154</v>
       </c>
       <c r="L107" t="n">
+        <v>5.67752198399209</v>
+      </c>
+      <c r="M107" t="n">
         <v>4</v>
       </c>
-      <c r="M107" t="n">
-        <v>1</v>
-      </c>
       <c r="N107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O107" t="n">
+        <v>1</v>
+      </c>
+      <c r="P107" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5452,15 +5776,18 @@
         <v>23.832756886468</v>
       </c>
       <c r="L108" t="n">
+        <v>3.43024071568898</v>
+      </c>
+      <c r="M108" t="n">
         <v>3</v>
       </c>
-      <c r="M108" t="n">
-        <v>2</v>
-      </c>
       <c r="N108" t="n">
         <v>2</v>
       </c>
       <c r="O108" t="n">
+        <v>1</v>
+      </c>
+      <c r="P108" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5499,15 +5826,18 @@
         <v>20.552750353668</v>
       </c>
       <c r="L109" t="n">
-        <v>2</v>
+        <v>1.90828361242247</v>
       </c>
       <c r="M109" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O109" t="n">
+        <v>1</v>
+      </c>
+      <c r="P109" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5546,16 +5876,19 @@
         <v>19.3292218559401</v>
       </c>
       <c r="L110" t="n">
-        <v>2</v>
+        <v>5.4875522740969</v>
       </c>
       <c r="M110" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O110" t="n">
         <v>1</v>
+      </c>
+      <c r="P110" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="111">
@@ -5593,15 +5926,18 @@
         <v>19.2663714600859</v>
       </c>
       <c r="L111" t="n">
+        <v>1.79173252285319</v>
+      </c>
+      <c r="M111" t="n">
         <v>3</v>
       </c>
-      <c r="M111" t="n">
-        <v>2</v>
-      </c>
       <c r="N111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O111" t="n">
+        <v>1</v>
+      </c>
+      <c r="P111" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5640,15 +5976,18 @@
         <v>36.4368682319029</v>
       </c>
       <c r="L112" t="n">
-        <v>3</v>
+        <v>-1.24423445304605</v>
       </c>
       <c r="M112" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O112" t="n">
+        <v>1</v>
+      </c>
+      <c r="P112" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5687,15 +6026,18 @@
         <v>30.3956987409221</v>
       </c>
       <c r="L113" t="n">
-        <v>4</v>
+        <v>1.38051324706529</v>
       </c>
       <c r="M113" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N113" t="n">
         <v>2</v>
       </c>
       <c r="O113" t="n">
+        <v>1</v>
+      </c>
+      <c r="P113" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5734,16 +6076,19 @@
         <v>24.8482497169627</v>
       </c>
       <c r="L114" t="n">
-        <v>4</v>
+        <v>0.46845763257144</v>
       </c>
       <c r="M114" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N114" t="n">
         <v>1</v>
       </c>
       <c r="O114" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P114" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -5781,15 +6126,18 @@
         <v>28.3232857262882</v>
       </c>
       <c r="L115" t="n">
+        <v>3.27935222009256</v>
+      </c>
+      <c r="M115" t="n">
         <v>4</v>
       </c>
-      <c r="M115" t="n">
-        <v>2</v>
-      </c>
       <c r="N115" t="n">
         <v>1</v>
       </c>
       <c r="O115" t="n">
+        <v>1</v>
+      </c>
+      <c r="P115" t="n">
         <v>2</v>
       </c>
     </row>
@@ -5828,15 +6176,18 @@
         <v>31.8669806508117</v>
       </c>
       <c r="L116" t="n">
-        <v>3</v>
+        <v>3.4970662255276</v>
       </c>
       <c r="M116" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N116" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O116" t="n">
+        <v>1</v>
+      </c>
+      <c r="P116" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5875,15 +6226,18 @@
         <v>25.3685215789583</v>
       </c>
       <c r="L117" t="n">
+        <v>3.5125582180863</v>
+      </c>
+      <c r="M117" t="n">
         <v>4</v>
       </c>
-      <c r="M117" t="n">
-        <v>2</v>
-      </c>
       <c r="N117" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O117" t="n">
+        <v>1</v>
+      </c>
+      <c r="P117" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5922,15 +6276,18 @@
         <v>30.7903321678547</v>
       </c>
       <c r="L118" t="n">
-        <v>4</v>
+        <v>-0.283199158351878</v>
       </c>
       <c r="M118" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N118" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O118" t="n">
+        <v>1</v>
+      </c>
+      <c r="P118" t="n">
         <v>1</v>
       </c>
     </row>
@@ -5969,15 +6326,18 @@
         <v>20.2174125741313</v>
       </c>
       <c r="L119" t="n">
+        <v>3.08605793125675</v>
+      </c>
+      <c r="M119" t="n">
         <v>3</v>
       </c>
-      <c r="M119" t="n">
-        <v>2</v>
-      </c>
       <c r="N119" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O119" t="n">
+        <v>1</v>
+      </c>
+      <c r="P119" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6016,15 +6376,18 @@
         <v>30.0269298605251</v>
       </c>
       <c r="L120" t="n">
-        <v>3</v>
+        <v>1.14814955796643</v>
       </c>
       <c r="M120" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N120" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O120" t="n">
+        <v>1</v>
+      </c>
+      <c r="P120" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6063,16 +6426,19 @@
         <v>24.4846935351049</v>
       </c>
       <c r="L121" t="n">
+        <v>3.95436616162471</v>
+      </c>
+      <c r="M121" t="n">
         <v>3</v>
       </c>
-      <c r="M121" t="n">
-        <v>2</v>
-      </c>
       <c r="N121" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O121" t="n">
         <v>1</v>
+      </c>
+      <c r="P121" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="122">
@@ -6110,15 +6476,18 @@
         <v>18.36167189294</v>
       </c>
       <c r="L122" t="n">
-        <v>2</v>
+        <v>3.0961128001959</v>
       </c>
       <c r="M122" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N122" t="n">
         <v>1</v>
       </c>
       <c r="O122" t="n">
+        <v>1</v>
+      </c>
+      <c r="P122" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6157,7 +6526,7 @@
         <v>36.289754406636</v>
       </c>
       <c r="L123" t="n">
-        <v>3</v>
+        <v>2.77479026649035</v>
       </c>
       <c r="M123" t="n">
         <v>2</v>
@@ -6166,6 +6535,9 @@
         <v>2</v>
       </c>
       <c r="O123" t="n">
+        <v>1</v>
+      </c>
+      <c r="P123" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6204,15 +6576,18 @@
         <v>22.2891751513476</v>
       </c>
       <c r="L124" t="n">
+        <v>5.86940603212744</v>
+      </c>
+      <c r="M124" t="n">
         <v>4</v>
       </c>
-      <c r="M124" t="n">
-        <v>2</v>
-      </c>
       <c r="N124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O124" t="n">
+        <v>2</v>
+      </c>
+      <c r="P124" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6251,15 +6626,18 @@
         <v>22.6692469917168</v>
       </c>
       <c r="L125" t="n">
-        <v>3</v>
+        <v>2.23804807319624</v>
       </c>
       <c r="M125" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N125" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O125" t="n">
+        <v>1</v>
+      </c>
+      <c r="P125" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6298,15 +6676,18 @@
         <v>37.8123563518618</v>
       </c>
       <c r="L126" t="n">
+        <v>0.717812226436815</v>
+      </c>
+      <c r="M126" t="n">
         <v>4</v>
       </c>
-      <c r="M126" t="n">
-        <v>2</v>
-      </c>
       <c r="N126" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O126" t="n">
+        <v>1</v>
+      </c>
+      <c r="P126" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6345,15 +6726,18 @@
         <v>20.2749691698544</v>
       </c>
       <c r="L127" t="n">
-        <v>3</v>
+        <v>0.355750435141708</v>
       </c>
       <c r="M127" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N127" t="n">
         <v>1</v>
       </c>
       <c r="O127" t="n">
+        <v>1</v>
+      </c>
+      <c r="P127" t="n">
         <v>2</v>
       </c>
     </row>
@@ -6392,15 +6776,18 @@
         <v>26.196650682316</v>
       </c>
       <c r="L128" t="n">
+        <v>4.99582060859343</v>
+      </c>
+      <c r="M128" t="n">
         <v>4</v>
       </c>
-      <c r="M128" t="n">
-        <v>2</v>
-      </c>
       <c r="N128" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O128" t="n">
+        <v>1</v>
+      </c>
+      <c r="P128" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6439,16 +6826,19 @@
         <v>28.1051020182228</v>
       </c>
       <c r="L129" t="n">
-        <v>3</v>
+        <v>3.20172321172182</v>
       </c>
       <c r="M129" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N129" t="n">
         <v>1</v>
       </c>
       <c r="O129" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P129" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="130">
@@ -6486,15 +6876,18 @@
         <v>25.487858962775</v>
       </c>
       <c r="L130" t="n">
-        <v>4</v>
+        <v>0.864200139996907</v>
       </c>
       <c r="M130" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O130" t="n">
+        <v>1</v>
+      </c>
+      <c r="P130" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6533,15 +6926,18 @@
         <v>19.6989379008042</v>
       </c>
       <c r="L131" t="n">
-        <v>3</v>
+        <v>0.458313800546378</v>
       </c>
       <c r="M131" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N131" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O131" t="n">
+        <v>1</v>
+      </c>
+      <c r="P131" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6580,15 +6976,18 @@
         <v>19.010608766134</v>
       </c>
       <c r="L132" t="n">
-        <v>3</v>
+        <v>2.15461106248753</v>
       </c>
       <c r="M132" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N132" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O132" t="n">
+        <v>1</v>
+      </c>
+      <c r="P132" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6627,15 +7026,18 @@
         <v>31.0524907861256</v>
       </c>
       <c r="L133" t="n">
+        <v>2.68233417387896</v>
+      </c>
+      <c r="M133" t="n">
         <v>3</v>
       </c>
-      <c r="M133" t="n">
-        <v>2</v>
-      </c>
       <c r="N133" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O133" t="n">
+        <v>2</v>
+      </c>
+      <c r="P133" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6674,15 +7076,18 @@
         <v>24.6858317960118</v>
       </c>
       <c r="L134" t="n">
-        <v>4</v>
+        <v>0.126902067133069</v>
       </c>
       <c r="M134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N134" t="n">
         <v>2</v>
       </c>
       <c r="O134" t="n">
+        <v>1</v>
+      </c>
+      <c r="P134" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6721,15 +7126,18 @@
         <v>31.7712233635063</v>
       </c>
       <c r="L135" t="n">
-        <v>4</v>
+        <v>5.25663668153289</v>
       </c>
       <c r="M135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N135" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O135" t="n">
+        <v>1</v>
+      </c>
+      <c r="P135" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6768,15 +7176,18 @@
         <v>32.3195720626988</v>
       </c>
       <c r="L136" t="n">
-        <v>4</v>
+        <v>3.32805526789172</v>
       </c>
       <c r="M136" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N136" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O136" t="n">
+        <v>1</v>
+      </c>
+      <c r="P136" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6815,15 +7226,18 @@
         <v>32.7345948015781</v>
       </c>
       <c r="L137" t="n">
-        <v>3</v>
+        <v>2.43452345878507</v>
       </c>
       <c r="M137" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N137" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O137" t="n">
+        <v>2</v>
+      </c>
+      <c r="P137" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6862,15 +7276,18 @@
         <v>24.4333864604973</v>
       </c>
       <c r="L138" t="n">
+        <v>2.73642696314862</v>
+      </c>
+      <c r="M138" t="n">
         <v>4</v>
       </c>
-      <c r="M138" t="n">
-        <v>2</v>
-      </c>
       <c r="N138" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O138" t="n">
+        <v>1</v>
+      </c>
+      <c r="P138" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6909,15 +7326,18 @@
         <v>34.8949796176209</v>
       </c>
       <c r="L139" t="n">
-        <v>2</v>
+        <v>3.24076993274976</v>
       </c>
       <c r="M139" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N139" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O139" t="n">
+        <v>1</v>
+      </c>
+      <c r="P139" t="n">
         <v>1</v>
       </c>
     </row>
@@ -6956,7 +7376,7 @@
         <v>25.4158697829075</v>
       </c>
       <c r="L140" t="n">
-        <v>4</v>
+        <v>1.80518867263432</v>
       </c>
       <c r="M140" t="n">
         <v>2</v>
@@ -6965,6 +7385,9 @@
         <v>2</v>
       </c>
       <c r="O140" t="n">
+        <v>1</v>
+      </c>
+      <c r="P140" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7003,16 +7426,19 @@
         <v>30.4055539245844</v>
       </c>
       <c r="L141" t="n">
+        <v>3.2904237166673</v>
+      </c>
+      <c r="M141" t="n">
         <v>3</v>
       </c>
-      <c r="M141" t="n">
-        <v>2</v>
-      </c>
       <c r="N141" t="n">
         <v>1</v>
       </c>
       <c r="O141" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P141" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="142">
@@ -7050,15 +7476,18 @@
         <v>27.0673737248232</v>
       </c>
       <c r="L142" t="n">
+        <v>3.50970653807692</v>
+      </c>
+      <c r="M142" t="n">
         <v>3</v>
       </c>
-      <c r="M142" t="n">
-        <v>2</v>
-      </c>
       <c r="N142" t="n">
         <v>2</v>
       </c>
       <c r="O142" t="n">
+        <v>1</v>
+      </c>
+      <c r="P142" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7097,16 +7526,19 @@
         <v>25.5569286191004</v>
       </c>
       <c r="L143" t="n">
+        <v>2.34648987918271</v>
+      </c>
+      <c r="M143" t="n">
         <v>3</v>
       </c>
-      <c r="M143" t="n">
-        <v>2</v>
-      </c>
       <c r="N143" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O143" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P143" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="144">
@@ -7144,15 +7576,18 @@
         <v>13.318865597406</v>
       </c>
       <c r="L144" t="n">
-        <v>3</v>
+        <v>0.632444595587474</v>
       </c>
       <c r="M144" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N144" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O144" t="n">
+        <v>1</v>
+      </c>
+      <c r="P144" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7191,16 +7626,19 @@
         <v>28.7867745971883</v>
       </c>
       <c r="L145" t="n">
+        <v>4.18099080081003</v>
+      </c>
+      <c r="M145" t="n">
         <v>3</v>
       </c>
-      <c r="M145" t="n">
-        <v>2</v>
-      </c>
       <c r="N145" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O145" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P145" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="146">
@@ -7238,15 +7676,18 @@
         <v>28.3501329463209</v>
       </c>
       <c r="L146" t="n">
+        <v>3.47272117801531</v>
+      </c>
+      <c r="M146" t="n">
         <v>4</v>
       </c>
-      <c r="M146" t="n">
-        <v>2</v>
-      </c>
       <c r="N146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O146" t="n">
+        <v>1</v>
+      </c>
+      <c r="P146" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7285,15 +7726,18 @@
         <v>26.7895216019753</v>
       </c>
       <c r="L147" t="n">
-        <v>2</v>
+        <v>1.33660405814917</v>
       </c>
       <c r="M147" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N147" t="n">
         <v>1</v>
       </c>
       <c r="O147" t="n">
+        <v>1</v>
+      </c>
+      <c r="P147" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7332,15 +7776,18 @@
         <v>28.8251729995963</v>
       </c>
       <c r="L148" t="n">
+        <v>0.621647331491768</v>
+      </c>
+      <c r="M148" t="n">
         <v>4</v>
       </c>
-      <c r="M148" t="n">
-        <v>2</v>
-      </c>
       <c r="N148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O148" t="n">
+        <v>1</v>
+      </c>
+      <c r="P148" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7379,16 +7826,19 @@
         <v>32.0695266638395</v>
       </c>
       <c r="L149" t="n">
-        <v>3</v>
+        <v>-0.0290428645905947</v>
       </c>
       <c r="M149" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N149" t="n">
         <v>1</v>
       </c>
       <c r="O149" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P149" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -7426,15 +7876,18 @@
         <v>25.4397589633302</v>
       </c>
       <c r="L150" t="n">
-        <v>2</v>
+        <v>2.94075426680955</v>
       </c>
       <c r="M150" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O150" t="n">
+        <v>1</v>
+      </c>
+      <c r="P150" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7473,15 +7926,18 @@
         <v>26.3373453033394</v>
       </c>
       <c r="L151" t="n">
-        <v>4</v>
+        <v>3.02575996491263</v>
       </c>
       <c r="M151" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N151" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O151" t="n">
+        <v>1</v>
+      </c>
+      <c r="P151" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7520,16 +7976,19 @@
         <v>25.1708530870493</v>
       </c>
       <c r="L152" t="n">
-        <v>4</v>
+        <v>2.41686250179098</v>
       </c>
       <c r="M152" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N152" t="n">
         <v>1</v>
       </c>
       <c r="O152" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P152" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -7567,15 +8026,18 @@
         <v>29.6861327915255</v>
       </c>
       <c r="L153" t="n">
-        <v>4</v>
+        <v>2.76532497726971</v>
       </c>
       <c r="M153" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N153" t="n">
         <v>2</v>
       </c>
       <c r="O153" t="n">
+        <v>1</v>
+      </c>
+      <c r="P153" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7614,15 +8076,18 @@
         <v>29.4865254197236</v>
       </c>
       <c r="L154" t="n">
-        <v>4</v>
+        <v>1.03247430877777</v>
       </c>
       <c r="M154" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N154" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O154" t="n">
+        <v>1</v>
+      </c>
+      <c r="P154" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7661,16 +8126,19 @@
         <v>24.0729731089704</v>
       </c>
       <c r="L155" t="n">
+        <v>2.96812082334816</v>
+      </c>
+      <c r="M155" t="n">
         <v>4</v>
       </c>
-      <c r="M155" t="n">
-        <v>2</v>
-      </c>
       <c r="N155" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O155" t="n">
         <v>1</v>
+      </c>
+      <c r="P155" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -7708,15 +8176,18 @@
         <v>31.8245389520258</v>
       </c>
       <c r="L156" t="n">
-        <v>4</v>
+        <v>2.88745311950442</v>
       </c>
       <c r="M156" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N156" t="n">
         <v>2</v>
       </c>
       <c r="O156" t="n">
+        <v>1</v>
+      </c>
+      <c r="P156" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7755,15 +8226,18 @@
         <v>23.7827532833758</v>
       </c>
       <c r="L157" t="n">
-        <v>4</v>
+        <v>2.28151160043667</v>
       </c>
       <c r="M157" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N157" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O157" t="n">
+        <v>1</v>
+      </c>
+      <c r="P157" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7802,16 +8276,19 @@
         <v>26.2837100222387</v>
       </c>
       <c r="L158" t="n">
+        <v>4.45959355730719</v>
+      </c>
+      <c r="M158" t="n">
         <v>4</v>
       </c>
-      <c r="M158" t="n">
-        <v>2</v>
-      </c>
       <c r="N158" t="n">
         <v>1</v>
       </c>
       <c r="O158" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="P158" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -7849,16 +8326,19 @@
         <v>29.3125497138465</v>
       </c>
       <c r="L159" t="n">
+        <v>2.84794582840866</v>
+      </c>
+      <c r="M159" t="n">
         <v>3</v>
       </c>
-      <c r="M159" t="n">
-        <v>2</v>
-      </c>
       <c r="N159" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O159" t="n">
         <v>1</v>
+      </c>
+      <c r="P159" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -7896,15 +8376,18 @@
         <v>21.9695506862434</v>
       </c>
       <c r="L160" t="n">
-        <v>3</v>
+        <v>1.5838353602178</v>
       </c>
       <c r="M160" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N160" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O160" t="n">
+        <v>1</v>
+      </c>
+      <c r="P160" t="n">
         <v>1</v>
       </c>
     </row>
@@ -7943,16 +8426,19 @@
         <v>38.2018282662286</v>
       </c>
       <c r="L161" t="n">
-        <v>2</v>
+        <v>-1.01839937092035</v>
       </c>
       <c r="M161" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N161" t="n">
         <v>2</v>
       </c>
       <c r="O161" t="n">
         <v>1</v>
+      </c>
+      <c r="P161" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="162">
@@ -7990,15 +8476,18 @@
         <v>29.0611906773255</v>
       </c>
       <c r="L162" t="n">
+        <v>4.76659600971219</v>
+      </c>
+      <c r="M162" t="n">
         <v>3</v>
       </c>
-      <c r="M162" t="n">
-        <v>2</v>
-      </c>
       <c r="N162" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O162" t="n">
+        <v>2</v>
+      </c>
+      <c r="P162" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>